<commit_message>
Added post-pres and DMV %
</commit_message>
<xml_diff>
--- a/combined.xlsx
+++ b/combined.xlsx
@@ -29,31 +29,31 @@
     <t>Unaffiliated</t>
   </si>
   <si>
-    <t>2008-1</t>
-  </si>
-  <si>
-    <t>2008-2</t>
-  </si>
-  <si>
-    <t>2008-3</t>
-  </si>
-  <si>
-    <t>2008-4</t>
-  </si>
-  <si>
-    <t>2008-5</t>
-  </si>
-  <si>
-    <t>2008-6</t>
-  </si>
-  <si>
-    <t>2008-7</t>
-  </si>
-  <si>
-    <t>2008-8</t>
-  </si>
-  <si>
-    <t>2008-9</t>
+    <t>2008-01</t>
+  </si>
+  <si>
+    <t>2008-02</t>
+  </si>
+  <si>
+    <t>2008-03</t>
+  </si>
+  <si>
+    <t>2008-04</t>
+  </si>
+  <si>
+    <t>2008-05</t>
+  </si>
+  <si>
+    <t>2008-06</t>
+  </si>
+  <si>
+    <t>2008-07</t>
+  </si>
+  <si>
+    <t>2008-08</t>
+  </si>
+  <si>
+    <t>2008-09</t>
   </si>
   <si>
     <t>2008-10</t>
@@ -65,31 +65,31 @@
     <t>2008-12</t>
   </si>
   <si>
-    <t>2009-1</t>
-  </si>
-  <si>
-    <t>2009-2</t>
-  </si>
-  <si>
-    <t>2009-3</t>
-  </si>
-  <si>
-    <t>2009-4</t>
-  </si>
-  <si>
-    <t>2009-5</t>
-  </si>
-  <si>
-    <t>2009-6</t>
-  </si>
-  <si>
-    <t>2009-7</t>
-  </si>
-  <si>
-    <t>2009-8</t>
-  </si>
-  <si>
-    <t>2009-9</t>
+    <t>2009-01</t>
+  </si>
+  <si>
+    <t>2009-02</t>
+  </si>
+  <si>
+    <t>2009-03</t>
+  </si>
+  <si>
+    <t>2009-04</t>
+  </si>
+  <si>
+    <t>2009-05</t>
+  </si>
+  <si>
+    <t>2009-06</t>
+  </si>
+  <si>
+    <t>2009-07</t>
+  </si>
+  <si>
+    <t>2009-08</t>
+  </si>
+  <si>
+    <t>2009-09</t>
   </si>
   <si>
     <t>2009-10</t>
@@ -101,31 +101,31 @@
     <t>2009-12</t>
   </si>
   <si>
-    <t>2010-1</t>
-  </si>
-  <si>
-    <t>2010-2</t>
-  </si>
-  <si>
-    <t>2010-3</t>
-  </si>
-  <si>
-    <t>2010-4</t>
-  </si>
-  <si>
-    <t>2010-5</t>
-  </si>
-  <si>
-    <t>2010-6</t>
-  </si>
-  <si>
-    <t>2010-7</t>
-  </si>
-  <si>
-    <t>2010-8</t>
-  </si>
-  <si>
-    <t>2010-9</t>
+    <t>2010-01</t>
+  </si>
+  <si>
+    <t>2010-02</t>
+  </si>
+  <si>
+    <t>2010-03</t>
+  </si>
+  <si>
+    <t>2010-04</t>
+  </si>
+  <si>
+    <t>2010-05</t>
+  </si>
+  <si>
+    <t>2010-06</t>
+  </si>
+  <si>
+    <t>2010-07</t>
+  </si>
+  <si>
+    <t>2010-08</t>
+  </si>
+  <si>
+    <t>2010-09</t>
   </si>
   <si>
     <t>2010-10</t>
@@ -137,31 +137,31 @@
     <t>2010-12</t>
   </si>
   <si>
-    <t>2011-1</t>
-  </si>
-  <si>
-    <t>2011-2</t>
-  </si>
-  <si>
-    <t>2011-3</t>
-  </si>
-  <si>
-    <t>2011-4</t>
-  </si>
-  <si>
-    <t>2011-5</t>
-  </si>
-  <si>
-    <t>2011-6</t>
-  </si>
-  <si>
-    <t>2011-7</t>
-  </si>
-  <si>
-    <t>2011-8</t>
-  </si>
-  <si>
-    <t>2011-9</t>
+    <t>2011-01</t>
+  </si>
+  <si>
+    <t>2011-02</t>
+  </si>
+  <si>
+    <t>2011-03</t>
+  </si>
+  <si>
+    <t>2011-04</t>
+  </si>
+  <si>
+    <t>2011-05</t>
+  </si>
+  <si>
+    <t>2011-06</t>
+  </si>
+  <si>
+    <t>2011-07</t>
+  </si>
+  <si>
+    <t>2011-08</t>
+  </si>
+  <si>
+    <t>2011-09</t>
   </si>
   <si>
     <t>2011-10</t>
@@ -173,31 +173,31 @@
     <t>2011-12</t>
   </si>
   <si>
-    <t>2012-1</t>
-  </si>
-  <si>
-    <t>2012-2</t>
-  </si>
-  <si>
-    <t>2012-3</t>
-  </si>
-  <si>
-    <t>2012-4</t>
-  </si>
-  <si>
-    <t>2012-5</t>
-  </si>
-  <si>
-    <t>2012-6</t>
-  </si>
-  <si>
-    <t>2012-7</t>
-  </si>
-  <si>
-    <t>2012-8</t>
-  </si>
-  <si>
-    <t>2012-9</t>
+    <t>2012-01</t>
+  </si>
+  <si>
+    <t>2012-02</t>
+  </si>
+  <si>
+    <t>2012-03</t>
+  </si>
+  <si>
+    <t>2012-04</t>
+  </si>
+  <si>
+    <t>2012-05</t>
+  </si>
+  <si>
+    <t>2012-06</t>
+  </si>
+  <si>
+    <t>2012-07</t>
+  </si>
+  <si>
+    <t>2012-08</t>
+  </si>
+  <si>
+    <t>2012-09</t>
   </si>
   <si>
     <t>2012-10</t>
@@ -209,31 +209,31 @@
     <t>2012-12</t>
   </si>
   <si>
-    <t>2013-1</t>
-  </si>
-  <si>
-    <t>2013-2</t>
-  </si>
-  <si>
-    <t>2013-3</t>
-  </si>
-  <si>
-    <t>2013-4</t>
-  </si>
-  <si>
-    <t>2013-5</t>
-  </si>
-  <si>
-    <t>2013-6</t>
-  </si>
-  <si>
-    <t>2013-7</t>
-  </si>
-  <si>
-    <t>2013-8</t>
-  </si>
-  <si>
-    <t>2013-9</t>
+    <t>2013-01</t>
+  </si>
+  <si>
+    <t>2013-02</t>
+  </si>
+  <si>
+    <t>2013-03</t>
+  </si>
+  <si>
+    <t>2013-04</t>
+  </si>
+  <si>
+    <t>2013-05</t>
+  </si>
+  <si>
+    <t>2013-06</t>
+  </si>
+  <si>
+    <t>2013-07</t>
+  </si>
+  <si>
+    <t>2013-08</t>
+  </si>
+  <si>
+    <t>2013-09</t>
   </si>
   <si>
     <t>2013-10</t>
@@ -245,31 +245,31 @@
     <t>2013-12</t>
   </si>
   <si>
-    <t>2014-1</t>
-  </si>
-  <si>
-    <t>2014-2</t>
-  </si>
-  <si>
-    <t>2014-3</t>
-  </si>
-  <si>
-    <t>2014-4</t>
-  </si>
-  <si>
-    <t>2014-5</t>
-  </si>
-  <si>
-    <t>2014-6</t>
-  </si>
-  <si>
-    <t>2014-7</t>
-  </si>
-  <si>
-    <t>2014-8</t>
-  </si>
-  <si>
-    <t>2014-9</t>
+    <t>2014-01</t>
+  </si>
+  <si>
+    <t>2014-02</t>
+  </si>
+  <si>
+    <t>2014-03</t>
+  </si>
+  <si>
+    <t>2014-04</t>
+  </si>
+  <si>
+    <t>2014-05</t>
+  </si>
+  <si>
+    <t>2014-06</t>
+  </si>
+  <si>
+    <t>2014-07</t>
+  </si>
+  <si>
+    <t>2014-08</t>
+  </si>
+  <si>
+    <t>2014-09</t>
   </si>
   <si>
     <t>2014-10</t>
@@ -281,31 +281,31 @@
     <t>2014-12</t>
   </si>
   <si>
-    <t>2015-1</t>
-  </si>
-  <si>
-    <t>2015-2</t>
-  </si>
-  <si>
-    <t>2015-3</t>
-  </si>
-  <si>
-    <t>2015-4</t>
-  </si>
-  <si>
-    <t>2015-5</t>
-  </si>
-  <si>
-    <t>2015-6</t>
-  </si>
-  <si>
-    <t>2015-7</t>
-  </si>
-  <si>
-    <t>2015-8</t>
-  </si>
-  <si>
-    <t>2015-9</t>
+    <t>2015-01</t>
+  </si>
+  <si>
+    <t>2015-02</t>
+  </si>
+  <si>
+    <t>2015-03</t>
+  </si>
+  <si>
+    <t>2015-04</t>
+  </si>
+  <si>
+    <t>2015-05</t>
+  </si>
+  <si>
+    <t>2015-06</t>
+  </si>
+  <si>
+    <t>2015-07</t>
+  </si>
+  <si>
+    <t>2015-08</t>
+  </si>
+  <si>
+    <t>2015-09</t>
   </si>
   <si>
     <t>2015-10</t>
@@ -317,31 +317,31 @@
     <t>2015-12</t>
   </si>
   <si>
-    <t>2016-1</t>
-  </si>
-  <si>
-    <t>2016-2</t>
-  </si>
-  <si>
-    <t>2016-3</t>
-  </si>
-  <si>
-    <t>2016-4</t>
-  </si>
-  <si>
-    <t>2016-5</t>
-  </si>
-  <si>
-    <t>2016-6</t>
-  </si>
-  <si>
-    <t>2016-7</t>
-  </si>
-  <si>
-    <t>2016-8</t>
-  </si>
-  <si>
-    <t>2016-9</t>
+    <t>2016-01</t>
+  </si>
+  <si>
+    <t>2016-02</t>
+  </si>
+  <si>
+    <t>2016-03</t>
+  </si>
+  <si>
+    <t>2016-04</t>
+  </si>
+  <si>
+    <t>2016-05</t>
+  </si>
+  <si>
+    <t>2016-06</t>
+  </si>
+  <si>
+    <t>2016-07</t>
+  </si>
+  <si>
+    <t>2016-08</t>
+  </si>
+  <si>
+    <t>2016-09</t>
   </si>
   <si>
     <t>2016-10</t>
@@ -353,31 +353,31 @@
     <t>2016-12</t>
   </si>
   <si>
-    <t>2017-1</t>
-  </si>
-  <si>
-    <t>2017-2</t>
-  </si>
-  <si>
-    <t>2017-3</t>
-  </si>
-  <si>
-    <t>2017-4</t>
-  </si>
-  <si>
-    <t>2017-5</t>
-  </si>
-  <si>
-    <t>2017-6</t>
-  </si>
-  <si>
-    <t>2017-7</t>
-  </si>
-  <si>
-    <t>2017-8</t>
-  </si>
-  <si>
-    <t>2017-9</t>
+    <t>2017-01</t>
+  </si>
+  <si>
+    <t>2017-02</t>
+  </si>
+  <si>
+    <t>2017-03</t>
+  </si>
+  <si>
+    <t>2017-04</t>
+  </si>
+  <si>
+    <t>2017-05</t>
+  </si>
+  <si>
+    <t>2017-06</t>
+  </si>
+  <si>
+    <t>2017-07</t>
+  </si>
+  <si>
+    <t>2017-08</t>
+  </si>
+  <si>
+    <t>2017-09</t>
   </si>
   <si>
     <t>2017-10</t>
@@ -389,22 +389,22 @@
     <t>2017-12</t>
   </si>
   <si>
-    <t>2018-1</t>
-  </si>
-  <si>
-    <t>2018-2</t>
-  </si>
-  <si>
-    <t>2018-3</t>
-  </si>
-  <si>
-    <t>2018-4</t>
-  </si>
-  <si>
-    <t>2018-5</t>
-  </si>
-  <si>
-    <t>2018-6</t>
+    <t>2018-01</t>
+  </si>
+  <si>
+    <t>2018-02</t>
+  </si>
+  <si>
+    <t>2018-03</t>
+  </si>
+  <si>
+    <t>2018-04</t>
+  </si>
+  <si>
+    <t>2018-05</t>
+  </si>
+  <si>
+    <t>2018-06</t>
   </si>
 </sst>
 </file>

</xml_diff>